<commit_message>
All the coding is finished.
Decision Tree is done.
All the models have been evaluated.
Everything is complete.
outliers checked.
Everything commented
</commit_message>
<xml_diff>
--- a/Things_To_Do_Checklist.xlsx
+++ b/Things_To_Do_Checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\6006\Course work\9789180-SI-s1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA81BAEC-266B-487C-8E8A-4839D1E18D2A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F73DC097-D4C9-4AA3-9840-F461E483B0A3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="25">
   <si>
     <t>URLs (dataset, Coventry GitHub, Coventry OneDrive-if needed)</t>
   </si>
@@ -93,7 +93,13 @@
     <t>Goals</t>
   </si>
   <si>
-    <t>Progress</t>
+    <t>Progress in code</t>
+  </si>
+  <si>
+    <t>Progress in report</t>
+  </si>
+  <si>
+    <t>Progress in video</t>
   </si>
 </sst>
 </file>
@@ -149,11 +155,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8D2AA940-E426-4090-B163-8ED4C578893A}" name="Table1" displayName="Table1" ref="A1:B24" totalsRowShown="0">
-  <autoFilter ref="A1:B24" xr:uid="{961E424C-F34F-4758-BAA4-66BB9736C710}"/>
-  <tableColumns count="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8D2AA940-E426-4090-B163-8ED4C578893A}" name="Table1" displayName="Table1" ref="A1:D24" totalsRowShown="0">
+  <autoFilter ref="A1:D24" xr:uid="{961E424C-F34F-4758-BAA4-66BB9736C710}"/>
+  <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{B08D1938-18BC-4357-A739-E047D5BDE1F2}" name="Goals"/>
-    <tableColumn id="2" xr3:uid="{C35BE1BE-77CF-4200-B32C-6F98C3640521}" name="Progress"/>
+    <tableColumn id="2" xr3:uid="{C35BE1BE-77CF-4200-B32C-6F98C3640521}" name="Progress in code"/>
+    <tableColumn id="3" xr3:uid="{EACFF4BD-B90D-45B4-B7D3-492F72D5CDFC}" name="Progress in report"/>
+    <tableColumn id="4" xr3:uid="{E340F3C3-AFE3-4C47-8DE7-F3B502A10A21}" name="Progress in video"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -422,72 +430,83 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B23"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="60.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.26953125" customWidth="1"/>
+    <col min="2" max="2" width="16.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>21</v>
       </c>
       <c r="B1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>3</v>
       </c>
-      <c r="B6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>4</v>
       </c>
-      <c r="B7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>5</v>
       </c>
-      <c r="B8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -495,7 +514,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -503,64 +522,79 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B16" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>13</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>14</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>15</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>16</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>17</v>
       </c>

</xml_diff>